<commit_message>
Evaporation Runs from last week
</commit_message>
<xml_diff>
--- a/2 - RiverWare Modeling/With Evaporation Modeling/Hydrology/Evap_Hist.xlsx
+++ b/2 - RiverWare Modeling/With Evaporation Modeling/Hydrology/Evap_Hist.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\WeberBasinVulnerability\WeberBasinVulnerability\2 - RiverWare Modeling\Hydrology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\WeberBasinVulnerability\WeberBasinVulnerability\2 - RiverWare Modeling\With Evaporation Modeling\Hydrology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC900144-DD82-42E8-BE08-09D183286CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DA41BD-9A27-45D6-BC1E-A8A95D436EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Run0" sheetId="1" r:id="rId1"/>
+    <sheet name="Trace2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -458,7 +458,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>